<commit_message>
Second example transcription (incomplete)
</commit_message>
<xml_diff>
--- a/data/trasncription_ex1.xlsx
+++ b/data/trasncription_ex1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/serenekim/Library/CloudStorage/OneDrive-VrijeUniversiteitBrussel/img-analysis_seorin_project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4C6EDF-694C-0B49-8199-BE0E614E8D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89EA9A68-0CFC-C247-B25A-C939E897A082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{6D6EFBF4-D3F9-A04D-9AC4-202B897D114E}"/>
   </bookViews>
@@ -314,9 +314,6 @@
     <t>14 avril 1920</t>
   </si>
   <si>
-    <t>Raoul Max</t>
-  </si>
-  <si>
     <t>d</t>
   </si>
   <si>
@@ -327,6 +324,9 @@
   </si>
   <si>
     <t>1 août 1919</t>
+  </si>
+  <si>
+    <t>Raoul Oscar</t>
   </si>
 </sst>
 </file>
@@ -904,7 +904,7 @@
   <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1106,7 +1106,7 @@
         <v>36</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
         <v>37</v>
@@ -1282,13 +1282,13 @@
         <v>400</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" t="s">
         <v>61</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E12" t="s">
         <v>62</v>
@@ -1312,10 +1312,10 @@
       <c r="L12" s="5"/>
       <c r="N12" s="4"/>
       <c r="O12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q12" s="5"/>
       <c r="S12" s="4"/>
@@ -1327,7 +1327,7 @@
         <v>401</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C13" t="s">
         <v>65</v>
@@ -1354,7 +1354,7 @@
       <c r="L13" s="5"/>
       <c r="N13" s="4"/>
       <c r="O13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P13" s="4" t="s">
         <v>69</v>
@@ -1423,7 +1423,7 @@
         <v>77</v>
       </c>
       <c r="O15" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P15" s="11" t="s">
         <v>78</v>

</xml_diff>